<commit_message>
buat costum layout chat and buat function chatbot history
</commit_message>
<xml_diff>
--- a/chatlog.xlsx
+++ b/chatlog.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,6 +485,25 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>apa tips untuk sukses</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalam belajar:
+1. Buatlah rencana belajar yang teratur: Buatlah rencana belajar yang teratur dan jelas. Rencana belajar ini harus mencakup jadwal belajar, materi yang akan dibahas, dan waktu yang akan digunakan untuk belajar.
+2. Carilah tempat yang nyaman dan tenang: Temukanlah tempat yang nyaman dan tenang untuk belajar. Pilihlah tempat yang tidak terlalu ramai dan tidak terlalu gelap.
+3. Lakukanlah pengulangan: Pengulangan adalah salah satu cara terbaik untuk mengingat informasi. Lakukanlah pengulangan dengan menuliskan informasi yang telah diajarkan dan membacanya kembali.
+4. Buatlah catatan: Tuliskanlah catatan-catatan penting yang diajarkan dan bacalah catatan-catatan tersebut setiap hari. Ini akan membantu Anda mengingat informasi yang telah dipelajari.
+5. Berdiskusilah dengan teman: Berdiskusilah dengan teman-teman Anda tentang materi yang telah dipelajari. Ini akan membantu Anda memahami informasi dengan lebih baik.
+6. Berlatihlah secara teratur: Berlatihlah materi yang telah dipelajari secara teratur. Ini akan membantu Anda menguasai materi dengan lebih baik.
+7. Jangan tunda-tunda pekerjaan: Jangan tunda-tunda pekerjaan yang telah diberikan. Ini akan membantu Anda menyelesaikan pekerjaan dengan lebih cepat dan membuat Anda lebih bersemangat untuk belajar.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>